<commit_message>
[맘파] StageTable 2-5 추가, Name칼럼 오타 수정
</commit_message>
<xml_diff>
--- a/ExcelConverter/ExcelFiles/StageTable.xlsx
+++ b/ExcelConverter/ExcelFiles/StageTable.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
   <si>
     <t>테이블 설명: 스테이지 관련 데이터를 관리 및 사용하기 위함</t>
   </si>
@@ -55,7 +55,7 @@
     <t>코멘트</t>
   </si>
   <si>
-    <t>NationID</t>
+    <t>ChapterID</t>
   </si>
   <si>
     <t>해당 스테이지가 속한 나라 ID</t>
@@ -132,28 +132,34 @@
     <t>stage1-5</t>
   </si>
   <si>
-    <t>Stage_Name_Use01</t>
+    <t>Stage_Name_Usa01</t>
   </si>
   <si>
     <t>stage2-1</t>
   </si>
   <si>
-    <t>Stage_Name_Use02</t>
+    <t>Stage_Name_Usa02</t>
   </si>
   <si>
     <t>stage2-2</t>
   </si>
   <si>
-    <t>Stage_Name_Use03</t>
+    <t>Stage_Name_Usa03</t>
   </si>
   <si>
     <t>stage2-3</t>
   </si>
   <si>
-    <t>Stage_Name_Use04</t>
+    <t>Stage_Name_Usa04</t>
   </si>
   <si>
     <t>stage2-4</t>
+  </si>
+  <si>
+    <t>Stage_Name_Usa05</t>
+  </si>
+  <si>
+    <t>stage2-5</t>
   </si>
 </sst>
 </file>
@@ -200,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -217,6 +223,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -439,7 +448,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="21.43"/>
-    <col customWidth="1" min="2" max="2" width="8.71"/>
+    <col customWidth="1" min="2" max="2" width="15.57"/>
     <col customWidth="1" min="3" max="3" width="53.43"/>
     <col customWidth="1" min="4" max="26" width="8.71"/>
   </cols>
@@ -475,9 +484,7 @@
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="2">
-        <v>44931.0</v>
-      </c>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" ht="16.5" customHeight="1">
       <c r="A9" s="1" t="s">
@@ -500,7 +507,7 @@
       </c>
     </row>
     <row r="11" ht="16.5" customHeight="1">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -520,9 +527,7 @@
       <c r="C12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="2">
-        <v>44958.0</v>
-      </c>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" ht="16.5" customHeight="1">
       <c r="A13" s="1" t="s">
@@ -533,9 +538,6 @@
       </c>
       <c r="C13" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="D13" s="5">
-        <v>1.0</v>
       </c>
     </row>
     <row r="14" ht="16.5" customHeight="1">
@@ -1587,7 +1589,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="8.71"/>
+    <col customWidth="1" min="1" max="1" width="8.71"/>
+    <col customWidth="1" min="2" max="2" width="17.29"/>
     <col customWidth="1" min="3" max="3" width="10.57"/>
     <col customWidth="1" min="4" max="10" width="8.71"/>
     <col customWidth="1" min="11" max="11" width="11.29"/>
@@ -1604,7 +1607,7 @@
       <c r="C1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -1840,7 +1843,7 @@
       <c r="A8" s="5">
         <v>6.0</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C8" s="2">
@@ -1875,7 +1878,7 @@
       <c r="A9" s="5">
         <v>7.0</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C9" s="2">
@@ -1910,7 +1913,7 @@
       <c r="A10" s="5">
         <v>8.0</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C10" s="2">
@@ -1945,7 +1948,7 @@
       <c r="A11" s="5">
         <v>9.0</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C11" s="2">
@@ -1955,7 +1958,7 @@
         <v>2.0</v>
       </c>
       <c r="E11" s="5">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="F11" s="5">
         <v>0.0</v>
@@ -1976,7 +1979,41 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" ht="16.5" customHeight="1"/>
+    <row r="12" ht="16.5" customHeight="1">
+      <c r="A12" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="2">
+        <v>45327.0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="G12" s="5">
+        <v>100.0</v>
+      </c>
+      <c r="H12" s="5">
+        <v>200.0</v>
+      </c>
+      <c r="I12" s="5">
+        <v>300.0</v>
+      </c>
+      <c r="J12" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="13" ht="16.5" customHeight="1"/>
     <row r="14" ht="16.5" customHeight="1"/>
     <row r="15" ht="16.5" customHeight="1"/>

</xml_diff>

<commit_message>
[맘파] StageTable StageTimer 칼럼 추가
</commit_message>
<xml_diff>
--- a/ExcelConverter/ExcelFiles/StageTable.xlsx
+++ b/ExcelConverter/ExcelFiles/StageTable.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
   <si>
     <t>테이블 설명: 스테이지 관련 데이터를 관리 및 사용하기 위함</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>스테이지 파일 연결</t>
+  </si>
+  <si>
+    <t>StageTimer</t>
+  </si>
+  <si>
+    <t>스테이지 제한 시간 [ 초 단위로 설정 ]</t>
   </si>
   <si>
     <t>StagePrefab</t>
@@ -584,7 +590,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" ht="16.5" customHeight="1"/>
+    <row r="18" ht="16.5" customHeight="1">
+      <c r="A18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="19" ht="16.5" customHeight="1"/>
     <row r="20" ht="16.5" customHeight="1"/>
     <row r="21" ht="16.5" customHeight="1"/>
@@ -1590,11 +1606,12 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="17.29"/>
+    <col customWidth="1" min="2" max="2" width="21.14"/>
     <col customWidth="1" min="3" max="3" width="10.57"/>
     <col customWidth="1" min="4" max="10" width="8.71"/>
     <col customWidth="1" min="11" max="11" width="11.29"/>
-    <col customWidth="1" min="12" max="29" width="8.71"/>
+    <col customWidth="1" min="12" max="12" width="10.71"/>
+    <col customWidth="1" min="13" max="29" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1">
@@ -1629,6 +1646,9 @@
         <v>24</v>
       </c>
       <c r="K1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1663,13 +1683,16 @@
       <c r="K2" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="L2" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" ht="16.5" customHeight="1">
       <c r="A3" s="5">
         <v>1.0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2">
         <v>44927.0</v>
@@ -1696,7 +1719,10 @@
         <v>0.0</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="L3" s="5">
+        <v>120.0</v>
       </c>
     </row>
     <row r="4" ht="16.5" customHeight="1">
@@ -1704,7 +1730,7 @@
         <v>2.0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C4" s="2">
         <v>44928.0</v>
@@ -1731,7 +1757,10 @@
         <v>0.0</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
+      </c>
+      <c r="L4" s="5">
+        <v>150.0</v>
       </c>
     </row>
     <row r="5" ht="16.5" customHeight="1">
@@ -1739,7 +1768,7 @@
         <v>3.0</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C5" s="2">
         <v>44929.0</v>
@@ -1766,7 +1795,10 @@
         <v>0.0</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="L5" s="5">
+        <v>240.0</v>
       </c>
     </row>
     <row r="6" ht="16.5" customHeight="1">
@@ -1774,7 +1806,7 @@
         <v>4.0</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C6" s="2">
         <v>44930.0</v>
@@ -1801,7 +1833,10 @@
         <v>0.0</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="L6" s="5">
+        <v>240.0</v>
       </c>
     </row>
     <row r="7" ht="16.5" customHeight="1">
@@ -1809,7 +1844,7 @@
         <v>5.0</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C7" s="2">
         <v>44931.0</v>
@@ -1836,7 +1871,10 @@
         <v>0.0</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="L7" s="5">
+        <v>420.0</v>
       </c>
     </row>
     <row r="8" ht="16.5" customHeight="1">
@@ -1844,7 +1882,7 @@
         <v>6.0</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2">
         <v>44958.0</v>
@@ -1871,7 +1909,10 @@
         <v>0.0</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="L8" s="5">
+        <v>210.0</v>
       </c>
     </row>
     <row r="9" ht="16.5" customHeight="1">
@@ -1879,7 +1920,7 @@
         <v>7.0</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C9" s="2">
         <v>44959.0</v>
@@ -1906,7 +1947,10 @@
         <v>0.0</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="L9" s="5">
+        <v>210.0</v>
       </c>
     </row>
     <row r="10" ht="16.5" customHeight="1">
@@ -1914,7 +1958,7 @@
         <v>8.0</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C10" s="2">
         <v>44960.0</v>
@@ -1941,7 +1985,10 @@
         <v>0.0</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="L10" s="5">
+        <v>210.0</v>
       </c>
     </row>
     <row r="11" ht="16.5" customHeight="1">
@@ -1949,7 +1996,7 @@
         <v>9.0</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C11" s="2">
         <v>44961.0</v>
@@ -1976,7 +2023,10 @@
         <v>0.0</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="L11" s="5">
+        <v>300.0</v>
       </c>
     </row>
     <row r="12" ht="16.5" customHeight="1">
@@ -1984,7 +2034,7 @@
         <v>10.0</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C12" s="2">
         <v>45327.0</v>
@@ -2011,7 +2061,10 @@
         <v>0.0</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="L12" s="5">
+        <v>420.0</v>
       </c>
     </row>
     <row r="13" ht="16.5" customHeight="1"/>

</xml_diff>